<commit_message>
Seperate bot commands add and /allusers added
</commit_message>
<xml_diff>
--- a/bot/data/users.xlsx
+++ b/bot/data/users.xlsx
@@ -428,39 +428,42 @@
     <row r="1" customFormat="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Telegram ID</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Full Name</t>
+          <t>username</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Username</t>
+          <t>user_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>created_at</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Umrbek Xudayorovich</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>username</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>user_id</t>
-        </is>
+          <t>pipcoder</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>324304236</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>created_at</t>
+          <t>2024-11-08T09:40:52.003144Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding cancel for /rekalama command and help modified for admin and users
</commit_message>
<xml_diff>
--- a/bot/data/users.xlsx
+++ b/bot/data/users.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,18 +450,38 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>dangoosh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>umrbek.xudayorovich@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1234567</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-11-08T10:02:47.978767Z</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>Umrbek Xudayorovich</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>pipcoder</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>324304236</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2024-11-08T09:40:52.003144Z</t>
         </is>

</xml_diff>